<commit_message>
added evaluation metrics nodes to the project
</commit_message>
<xml_diff>
--- a/project/core/nodes/schema.xlsx
+++ b/project/core/nodes/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406469B1-8CB0-4965-AAEC-A7F6F8DA0948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E7ABAB-79BE-4BA2-8632-D6A8A83BFFFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="126">
   <si>
     <t>node_name</t>
   </si>
@@ -406,6 +406,21 @@
   </si>
   <si>
     <t>["X","y"]</t>
+  </si>
+  <si>
+    <t>evluator</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>evaluate</t>
+  </si>
+  <si>
+    <t>["y_true","y_pred"]</t>
+  </si>
+  <si>
+    <t>["score"]</t>
   </si>
 </sst>
 </file>
@@ -482,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -498,6 +513,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -836,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2078,23 +2096,46 @@
       <c r="A54" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B54" s="8" t="s">
+      <c r="B54" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="8" t="s">
+      <c r="D54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="G54" s="6" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some modifications of evaluator logic & svm nodes display
</commit_message>
<xml_diff>
--- a/project/core/nodes/schema.xlsx
+++ b/project/core/nodes/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF226A8C-70C9-4010-867E-448BD8B6528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44628C4-43DA-48B4-A2DF-2DBF1D1BFA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="261">
   <si>
     <t>node_name</t>
   </si>
@@ -121,10 +121,6 @@
 {"name":"l1_ratio", "type":"float", "default":0.5}]</t>
   </si>
   <si>
-    <t>[{"name":"C", "type":"float", "default":1.0},
-{"name":"kernel", "type":"str", "default":"rbf"}]</t>
-  </si>
-  <si>
     <t>[{"name":"penalty", "type":"str", "default":"l2"}]</t>
   </si>
   <si>
@@ -441,10 +437,6 @@
   </si>
   <si>
     <t>[{"name":"C", "type":"float", "default":1.0},
-{"name":"kernel", "type":"str", "default":"poly"}]</t>
-  </si>
-  <si>
-    <t>[{"name":"C", "type":"float", "default":1.0},
 {"name":"kernel", "type":"str", "default":"sigmoid"}]</t>
   </si>
   <si>
@@ -830,6 +822,9 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>[{"name":"metric", "type":"str","default":"accuracy"}]</t>
   </si>
 </sst>
 </file>
@@ -1236,8 +1231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1257,16 +1252,16 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -1281,27 +1276,27 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -1322,21 +1317,21 @@
         <v>5</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>23</v>
@@ -1357,21 +1352,21 @@
         <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>22</v>
@@ -1392,21 +1387,21 @@
         <v>5</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>21</v>
@@ -1427,21 +1422,21 @@
         <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>20</v>
@@ -1453,7 +1448,7 @@
         <v>7</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>4</v>
@@ -1462,21 +1457,21 @@
         <v>5</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
@@ -1497,21 +1492,21 @@
         <v>5</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>18</v>
@@ -1532,21 +1527,21 @@
         <v>5</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>17</v>
@@ -1558,7 +1553,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>4</v>
@@ -1567,24 +1562,24 @@
         <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>9</v>
@@ -1593,7 +1588,7 @@
         <v>7</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>4</v>
@@ -1602,21 +1597,21 @@
         <v>5</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -1628,7 +1623,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>4</v>
@@ -1637,21 +1632,21 @@
         <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>12</v>
@@ -1663,7 +1658,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>4</v>
@@ -1672,21 +1667,21 @@
         <v>5</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>13</v>
@@ -1698,7 +1693,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>4</v>
@@ -1707,24 +1702,24 @@
         <v>5</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>9</v>
@@ -1733,7 +1728,7 @@
         <v>8</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>4</v>
@@ -1742,21 +1737,21 @@
         <v>5</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
@@ -1768,7 +1763,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>4</v>
@@ -1777,21 +1772,21 @@
         <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B16" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>15</v>
@@ -1803,7 +1798,7 @@
         <v>8</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>132</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>4</v>
@@ -1812,21 +1807,21 @@
         <v>5</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>16</v>
@@ -1838,7 +1833,7 @@
         <v>8</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>4</v>
@@ -1847,33 +1842,33 @@
         <v>5</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>4</v>
@@ -1882,33 +1877,33 @@
         <v>5</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>4</v>
@@ -1917,33 +1912,33 @@
         <v>5</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>4</v>
@@ -1952,33 +1947,33 @@
         <v>5</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>4</v>
@@ -1987,27 +1982,27 @@
         <v>5</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>7</v>
@@ -2022,27 +2017,27 @@
         <v>5</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>8</v>
@@ -2057,27 +2052,27 @@
         <v>5</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>7</v>
@@ -2092,27 +2087,27 @@
         <v>5</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B25" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>8</v>
@@ -2127,27 +2122,27 @@
         <v>5</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B26" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>7</v>
@@ -2162,27 +2157,27 @@
         <v>5</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B27" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>8</v>
@@ -2197,27 +2192,27 @@
         <v>5</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>8</v>
@@ -2232,27 +2227,27 @@
         <v>5</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>8</v>
@@ -2267,27 +2262,27 @@
         <v>5</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B30" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>8</v>
@@ -2302,33 +2297,33 @@
         <v>5</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B31" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>4</v>
@@ -2337,33 +2332,33 @@
         <v>5</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>8</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>4</v>
@@ -2372,100 +2367,100 @@
         <v>5</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B33" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="I33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B35" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>4</v>
@@ -2474,103 +2469,103 @@
         <v>4</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B36" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B37" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="H37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>4</v>
@@ -2579,33 +2574,33 @@
         <v>4</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>4</v>
@@ -2614,33 +2609,33 @@
         <v>4</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>4</v>
@@ -2649,33 +2644,33 @@
         <v>4</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B41" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E41" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="G41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>4</v>
@@ -2684,33 +2679,33 @@
         <v>4</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B42" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C42" s="1">
         <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>4</v>
@@ -2719,33 +2714,33 @@
         <v>4</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B43" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>4</v>
@@ -2754,33 +2749,33 @@
         <v>4</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B44" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>4</v>
@@ -2789,244 +2784,244 @@
         <v>4</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B45" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C45" s="1">
         <v>4</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B46" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="H46" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B47" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C47" s="1">
         <v>4</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B48" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C48" s="1">
         <v>4</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E48" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F48" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="H48" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B49" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B50" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C50" s="1">
         <v>5</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="H50" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G51" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="H51" s="1" t="s">
         <v>4</v>
       </c>
@@ -3034,69 +3029,69 @@
         <v>4</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B52" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E52" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G52" s="1" t="s">
+      <c r="H52" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I52" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H52" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="J52" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B53" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H53" s="1" t="s">
         <v>4</v>
       </c>
@@ -3104,115 +3099,115 @@
         <v>4</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B54" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C54" s="1">
         <v>5</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E54" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F54" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="H54" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="K54" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B55" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C55" s="1">
         <v>4</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="H55" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I55" s="1" t="s">
+      <c r="J55" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>106</v>
-      </c>
       <c r="K55" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B56" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E56" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H56" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H56" s="6" t="s">
+      <c r="I56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="I56" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="J56" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K56" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new line for description of component table for a better view
</commit_message>
<xml_diff>
--- a/project/core/nodes/schema.xlsx
+++ b/project/core/nodes/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44628C4-43DA-48B4-A2DF-2DBF1D1BFA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD8316B-09BF-4925-BC28-FB88B7E7952F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -656,175 +656,232 @@
     <t>["fitted_model","X"]</t>
   </si>
   <si>
-    <t>A simple regression model that fits a linear relationship between the input features and the target variable.</t>
-  </si>
-  <si>
-    <t>A linear regression model with L2 regularization to prevent overfitting by penalizing large coefficients.</t>
-  </si>
-  <si>
-    <t>A linear regression model with L1 regularization that encourages sparsity by setting some coefficients to zero.</t>
-  </si>
-  <si>
-    <t>A combination of L1 (Lasso) and L2 (Ridge) regularization to balance feature selection and shrinkage.</t>
-  </si>
-  <si>
-    <t>A linear regression model trained using Stochastic Gradient Descent (SGD) for large-scale datasets.</t>
-  </si>
-  <si>
-    <t>A Support Vector Regression model with a radial basis function (RBF) kernel, capturing complex non-linear relationships.</t>
-  </si>
-  <si>
-    <t>A Support Vector Regression model using a linear kernel for simple relationships.</t>
-  </si>
-  <si>
-    <t>A Support Vector Regression model with a polynomial kernel to capture non-linear dependencies.</t>
-  </si>
-  <si>
-    <t>A Support Vector Regression model with a sigmoid kernel, often used in specialized cases.</t>
-  </si>
-  <si>
-    <t>A non-linear regression model that splits data into hierarchical decision rules.</t>
-  </si>
-  <si>
-    <t>An ensemble method that combines multiple decision trees to improve prediction accuracy.</t>
-  </si>
-  <si>
-    <t>A boosting model that sequentially improves weak decision trees for enhanced predictive performance.</t>
-  </si>
-  <si>
-    <t>A boosting method that adjusts weak models iteratively to minimize errors.</t>
-  </si>
-  <si>
-    <t>An ensemble method that trains multiple instances of a regression model on different data samples for robustness.</t>
-  </si>
-  <si>
-    <t>A non-parametric regression model that predicts a target value based on the average of the k-nearest data points.</t>
-  </si>
-  <si>
-    <t>A linear classifier that estimates probabilities using the logistic function for binary classification.</t>
-  </si>
-  <si>
-    <t>A Ridge-regularized version of logistic regression to improve generalization.</t>
-  </si>
-  <si>
-    <t>A linear classifier trained using Stochastic Gradient Descent (SGD) for large-scale datasets.</t>
-  </si>
-  <si>
-    <t>A Support Vector Classification model using a linear kernel for simple classification tasks.</t>
-  </si>
-  <si>
-    <t>A Support Vector Classification model with an RBF kernel, capturing non-linear relationships.</t>
-  </si>
-  <si>
-    <t>A Support Vector Classification model using a polynomial kernel for complex decision boundaries.</t>
-  </si>
-  <si>
-    <t>A Support Vector Classification model with a sigmoid kernel, suitable for specific tasks.</t>
-  </si>
-  <si>
-    <t>A non-linear classifier that splits data based on feature values to make decisions.</t>
-  </si>
-  <si>
-    <t>An ensemble method that aggregates multiple decision trees to improve accuracy and reduce overfitting.</t>
-  </si>
-  <si>
-    <t>A boosting model that sequentially improves weak classifiers for better performance.</t>
-  </si>
-  <si>
-    <t>A boosting method that assigns more weight to misclassified instances in successive models.</t>
-  </si>
-  <si>
-    <t>An ensemble method that improves model stability by training classifiers on different random data subsets.</t>
-  </si>
-  <si>
-    <t>A probabilistic classifier that assumes normal distribution of feature values and independence between them.</t>
-  </si>
-  <si>
-    <t>A variant of Naïve Bayes suitable for discrete features like word counts in text classification.</t>
-  </si>
-  <si>
-    <t>A Naïve Bayes model designed for binary/boolean feature data.</t>
-  </si>
-  <si>
-    <t>A non-parametric classification model that assigns a label based on the majority vote of k-nearest data points.</t>
-  </si>
-  <si>
-    <t>Standardizes features by removing the mean and scaling to unit variance (Z-score normalization).</t>
-  </si>
-  <si>
-    <t>Scales features to a fixed range (default [0,1]) by transforming each value proportionally.</t>
-  </si>
-  <si>
-    <t>Scales each feature by its maximum absolute value, preserving the sign and keeping values between -1 and 1.</t>
-  </si>
-  <si>
-    <t>Uses median and interquartile range (IQR) for scaling, making it resistant to outliers.</t>
-  </si>
-  <si>
-    <t>Scales individual samples to have unit norm, useful for distance-based models like KNN and SVM.</t>
-  </si>
-  <si>
-    <t>Converts categorical labels into numeric values (e.g., ‘red’, ‘blue’, ‘green’ → 0, 1, 2).</t>
-  </si>
-  <si>
-    <t>Converts categorical values into binary columns, creating a separate column for each unique category.</t>
-  </si>
-  <si>
-    <t>Encodes categorical values as ordinal numbers (useful when categories have an inherent order).</t>
-  </si>
-  <si>
-    <t>Converts multi-class labels into binary (one-vs-rest) format for classification tasks.</t>
-  </si>
-  <si>
-    <t>Replaces missing values with a specified strategy (e.g., mean, median, most frequent).</t>
-  </si>
-  <si>
-    <t>Uses k-nearest neighbors to fill in missing values based on similar samples.</t>
-  </si>
-  <si>
-    <t>Converts numeric values into binary format based on a threshold (e.g., all values &gt;0.5 become 1, else 0).</t>
-  </si>
-  <si>
-    <t>A general utility that trains a machine learning model on a dataset.</t>
-  </si>
-  <si>
-    <t>Uses a trained model to make predictions on new data.</t>
-  </si>
-  <si>
-    <t>Fits a preprocessing step (e.g., scaling, encoding) to the dataset before applying transformations.</t>
-  </si>
-  <si>
-    <t>Applies transformations like scaling, encoding, or feature engineering to modify the dataset.</t>
-  </si>
-  <si>
-    <t>A combined step that both fits and transforms data in one go, useful in pipelines.</t>
-  </si>
-  <si>
-    <t>Divides data into separate subsets, such as training and testing sets.</t>
-  </si>
-  <si>
-    <t>Loads data from various sources (CSV, database, API, etc.) for use in machine learning models.</t>
-  </si>
-  <si>
-    <t>Saves processed data or model states into a structured format (e.g., JSON, database, file system).</t>
-  </si>
-  <si>
-    <t>Loads saved node data for reuse in machine learning workflows.</t>
-  </si>
-  <si>
-    <t>Merges datasets or data frames based on common attributes, useful for data preprocessing.</t>
-  </si>
-  <si>
-    <t>Assesses model performance using metrics such as accuracy, precision, recall, RMSE, etc.</t>
-  </si>
-  <si>
-    <t>Splits data into training and testing sets to validate model performance.</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
     <t>[{"name":"metric", "type":"str","default":"accuracy"}]</t>
+  </si>
+  <si>
+    <t>A simple regression model that fits a linear
+ relationship between the input features and the
+ target variable.</t>
+  </si>
+  <si>
+    <t>A linear regression model with L2 regularization 
+to prevent overfitting by penalizing large coefficients.</t>
+  </si>
+  <si>
+    <t>A linear regression model with L1 regularization 
+that encourages sparsity by setting some coefficients to zero.</t>
+  </si>
+  <si>
+    <t>A combination of L1 (Lasso) and L2 (Ridge) 
+regularization to balance feature selection and shrinkage.</t>
+  </si>
+  <si>
+    <t>A linear regression model trained using
+ Stochastic Gradient Descent (SGD) for large-scale datasets.</t>
+  </si>
+  <si>
+    <t>A linear classifier that estimates probabilities 
+using the logistic function for binary
+classification.</t>
+  </si>
+  <si>
+    <t>A Ridge-regularized version of logistic 
+regression to improve generalization.</t>
+  </si>
+  <si>
+    <t>Splits data into training and testing sets to 
+validate model performance.</t>
+  </si>
+  <si>
+    <t>Assesses model performance using metrics 
+such as accuracy, precision, recall, RMSE, etc.</t>
+  </si>
+  <si>
+    <t>Merges datasets or data frames based on 
+common attributes, useful for data preprocessing.</t>
+  </si>
+  <si>
+    <t>Loads saved node data for reuse in machine 
+learning workflows.</t>
+  </si>
+  <si>
+    <t>Saves processed data or model states into a 
+structured format (e.g., JSON, database, file system).</t>
+  </si>
+  <si>
+    <t>Loads data from various sources (CSV, 
+database, API, etc.) for use in machine learning models.</t>
+  </si>
+  <si>
+    <t>Divides data into separate subsets, such as 
+training and testing sets.</t>
+  </si>
+  <si>
+    <t>A combined step that both fits and transforms 
+data in one go, useful in pipelines.</t>
+  </si>
+  <si>
+    <t>Applies transformations like scaling, encoding, 
+or feature engineering to modify the dataset.</t>
+  </si>
+  <si>
+    <t>Fits a preprocessing step (e.g., scaling, 
+encoding) to the dataset before applying transformations.</t>
+  </si>
+  <si>
+    <t>Uses a trained model to make predictions on 
+new data.</t>
+  </si>
+  <si>
+    <t>A general utility that trains a machine learning 
+model on a dataset.</t>
+  </si>
+  <si>
+    <t>Converts numeric values into binary format 
+based on a threshold (e.g., all values &gt;0.5 become 1, else 0).</t>
+  </si>
+  <si>
+    <t>Uses k-nearest neighbors to fill in missing 
+values based on similar samples.</t>
+  </si>
+  <si>
+    <t>Replaces missing values with a specified 
+strategy (e.g., mean, median, most frequent).</t>
+  </si>
+  <si>
+    <t>Converts multi-class labels into binary (one-
+vs-rest) format for classification tasks.</t>
+  </si>
+  <si>
+    <t>Encodes categorical values as ordinal numbers 
+(useful when categories have an inherent order).</t>
+  </si>
+  <si>
+    <t>Converts categorical values into binary 
+columns, creating a separate column for each unique category.</t>
+  </si>
+  <si>
+    <t>Converts categorical labels into numeric 
+values (e.g., ‘red’, ‘blue’, ‘green’ → 0, 1, 2).</t>
+  </si>
+  <si>
+    <t>Scales individual samples to have unit norm, 
+useful for distance-based models like KNN and SVM.</t>
+  </si>
+  <si>
+    <t>Uses median and interquartile range (IQR) for 
+scaling, making it resistant to outliers.</t>
+  </si>
+  <si>
+    <t>Scales each feature by its maximum absolute 
+value, preserving the sign and keeping values between -1 and 1.</t>
+  </si>
+  <si>
+    <t>Scales features to a fixed range (default [0,1]) 
+by transforming each value proportionally.</t>
+  </si>
+  <si>
+    <t>Standardizes features by removing the mean 
+and scaling to unit variance (Z-score normalization).</t>
+  </si>
+  <si>
+    <t>A non-parametric classification model that 
+assigns a label based on the majority vote of k-nearest data points.</t>
+  </si>
+  <si>
+    <t>A non-parametric regression model that 
+predicts a target value based on the average of the k-nearest data points.</t>
+  </si>
+  <si>
+    <t>A Naïve Bayes model designed for binary/
+boolean feature data.</t>
+  </si>
+  <si>
+    <t>A variant of Naïve Bayes suitable for discrete 
+features like word counts in text classification.</t>
+  </si>
+  <si>
+    <t>A probabilistic classifier that assumes normal 
+distribution of feature values and independence between them.</t>
+  </si>
+  <si>
+    <t>An ensemble method that improves model 
+stability by training classifiers on different random data subsets.</t>
+  </si>
+  <si>
+    <t>An ensemble method that trains multiple 
+instances of a regression model on different data samples for robustness.</t>
+  </si>
+  <si>
+    <t>A boosting method that assigns more weight to 
+misclassified instances in successive models.</t>
+  </si>
+  <si>
+    <t>A linear classifier trained using Stochastic 
+Gradient Descent (SGD) for large-scale datasets.</t>
+  </si>
+  <si>
+    <t>A Support Vector Regression model with a 
+radial basis function (RBF) kernel, capturing complex non-linear relationships.</t>
+  </si>
+  <si>
+    <t>A Support Vector Regression model using a 
+linear kernel for simple relationships.</t>
+  </si>
+  <si>
+    <t>A Support Vector Regression model with a 
+polynomial kernel to capture non-linear dependencies.</t>
+  </si>
+  <si>
+    <t>A Support Vector Regression model with a 
+sigmoid kernel, often used in specialized cases.</t>
+  </si>
+  <si>
+    <t>A Support Vector Classification model using
+ a linear kernel for simple classification tasks.</t>
+  </si>
+  <si>
+    <t>A Support Vector Classification model with 
+an RBF kernel, capturing non-linear relationships.</t>
+  </si>
+  <si>
+    <t>A Support Vector Classification model using 
+a polynomial kernel for complex decision boundaries.</t>
+  </si>
+  <si>
+    <t>A Support Vector Classification model with a 
+sigmoid kernel, suitable for specific tasks.</t>
+  </si>
+  <si>
+    <t>A non-linear regression model that splits data 
+into hierarchical decision rules.</t>
+  </si>
+  <si>
+    <t>A non-linear classifier that splits data based on 
+feature values to make decisions.</t>
+  </si>
+  <si>
+    <t>An ensemble method that combines multiple 
+decision trees to improve prediction accuracy.</t>
+  </si>
+  <si>
+    <t>An ensemble method that aggregates multiple 
+decision trees to improve accuracy and reduce overfitting.</t>
+  </si>
+  <si>
+    <t>A boosting model that sequentially improves 
+weak decision trees for enhanced predictive performance.</t>
+  </si>
+  <si>
+    <t>A boosting model that sequentially improves 
+weak classifiers for better performance.</t>
+  </si>
+  <si>
+    <t>A boosting method that adjusts weak models 
+iteratively to minimize errors.</t>
   </si>
 </sst>
 </file>
@@ -875,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -894,6 +951,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,14 +1291,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="2" max="2" width="38.08984375" customWidth="1"/>
     <col min="3" max="3" width="5.54296875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
@@ -1255,7 +1315,7 @@
         <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>204</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>200</v>
@@ -1285,12 +1345,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B2" t="s">
-        <v>204</v>
+      <c r="B2" s="7" t="s">
+        <v>206</v>
       </c>
       <c r="C2" s="1">
         <v>2</v>
@@ -1320,12 +1380,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B3" t="s">
-        <v>205</v>
+      <c r="B3" s="7" t="s">
+        <v>207</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1355,12 +1415,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B4" t="s">
-        <v>206</v>
+      <c r="B4" s="7" t="s">
+        <v>208</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1390,12 +1450,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
-        <v>207</v>
+      <c r="B5" s="7" t="s">
+        <v>209</v>
       </c>
       <c r="C5" s="1">
         <v>2</v>
@@ -1425,12 +1485,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B6" t="s">
-        <v>208</v>
+      <c r="B6" s="7" t="s">
+        <v>210</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
@@ -1460,12 +1520,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B7" t="s">
-        <v>219</v>
+      <c r="B7" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1495,12 +1555,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B8" t="s">
-        <v>220</v>
+      <c r="B8" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1530,12 +1590,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="B9" t="s">
-        <v>221</v>
+      <c r="B9" s="7" t="s">
+        <v>245</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1565,12 +1625,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B10" t="s">
-        <v>209</v>
+      <c r="B10" s="7" t="s">
+        <v>246</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1600,12 +1660,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B11" t="s">
-        <v>210</v>
+      <c r="B11" s="7" t="s">
+        <v>247</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1635,12 +1695,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B12" t="s">
-        <v>211</v>
+      <c r="B12" s="7" t="s">
+        <v>248</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1670,12 +1730,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B13" t="s">
-        <v>212</v>
+      <c r="B13" s="7" t="s">
+        <v>249</v>
       </c>
       <c r="C13" s="1">
         <v>2</v>
@@ -1705,12 +1765,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B14" t="s">
-        <v>222</v>
+      <c r="B14" s="7" t="s">
+        <v>250</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1740,12 +1800,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B15" t="s">
-        <v>223</v>
+      <c r="B15" s="7" t="s">
+        <v>251</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -1775,12 +1835,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B16" t="s">
-        <v>224</v>
+      <c r="B16" s="7" t="s">
+        <v>252</v>
       </c>
       <c r="C16" s="1">
         <v>2</v>
@@ -1814,8 +1874,8 @@
       <c r="A17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B17" t="s">
-        <v>225</v>
+      <c r="B17" s="7" t="s">
+        <v>253</v>
       </c>
       <c r="C17" s="1">
         <v>2</v>
@@ -1845,12 +1905,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B18" t="s">
-        <v>213</v>
+      <c r="B18" s="7" t="s">
+        <v>254</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -1880,12 +1940,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B19" t="s">
-        <v>226</v>
+      <c r="B19" s="7" t="s">
+        <v>255</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1915,12 +1975,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B20" t="s">
-        <v>214</v>
+      <c r="B20" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="C20" s="1">
         <v>2</v>
@@ -1950,12 +2010,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B21" t="s">
-        <v>227</v>
+      <c r="B21" s="7" t="s">
+        <v>257</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -1985,12 +2045,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B22" t="s">
-        <v>215</v>
+      <c r="B22" s="7" t="s">
+        <v>258</v>
       </c>
       <c r="C22" s="1">
         <v>2</v>
@@ -2020,12 +2080,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B23" t="s">
-        <v>228</v>
+      <c r="B23" s="7" t="s">
+        <v>259</v>
       </c>
       <c r="C23" s="1">
         <v>2</v>
@@ -2055,12 +2115,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B24" t="s">
-        <v>216</v>
+      <c r="B24" s="7" t="s">
+        <v>260</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -2090,12 +2150,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B25" t="s">
-        <v>229</v>
+      <c r="B25" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -2125,12 +2185,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B26" t="s">
-        <v>217</v>
+      <c r="B26" s="7" t="s">
+        <v>243</v>
       </c>
       <c r="C26" s="1">
         <v>2</v>
@@ -2160,12 +2220,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B27" t="s">
-        <v>230</v>
+      <c r="B27" s="7" t="s">
+        <v>242</v>
       </c>
       <c r="C27" s="1">
         <v>2</v>
@@ -2195,12 +2255,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="B28" t="s">
-        <v>231</v>
+      <c r="B28" s="7" t="s">
+        <v>241</v>
       </c>
       <c r="C28" s="1">
         <v>2</v>
@@ -2230,12 +2290,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B29" t="s">
-        <v>232</v>
+      <c r="B29" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="C29" s="1">
         <v>2</v>
@@ -2265,12 +2325,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B30" t="s">
-        <v>233</v>
+      <c r="B30" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
@@ -2300,12 +2360,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B31" t="s">
-        <v>218</v>
+      <c r="B31" s="7" t="s">
+        <v>238</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -2335,12 +2395,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="B32" t="s">
-        <v>234</v>
+      <c r="B32" s="7" t="s">
+        <v>237</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -2370,12 +2430,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B33" t="s">
-        <v>235</v>
+      <c r="B33" s="7" t="s">
+        <v>236</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
@@ -2405,12 +2465,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B34" t="s">
-        <v>236</v>
+      <c r="B34" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
@@ -2440,12 +2500,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B35" t="s">
-        <v>237</v>
+      <c r="B35" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="C35" s="1">
         <v>3</v>
@@ -2475,12 +2535,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B36" t="s">
-        <v>238</v>
+      <c r="B36" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
@@ -2510,12 +2570,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B37" t="s">
-        <v>239</v>
+      <c r="B37" s="7" t="s">
+        <v>232</v>
       </c>
       <c r="C37" s="1">
         <v>3</v>
@@ -2545,12 +2605,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="B38" t="s">
-        <v>240</v>
+      <c r="B38" s="7" t="s">
+        <v>231</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
@@ -2580,12 +2640,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B39" t="s">
-        <v>241</v>
+      <c r="B39" s="7" t="s">
+        <v>230</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
@@ -2615,12 +2675,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B40" t="s">
-        <v>242</v>
+      <c r="B40" s="7" t="s">
+        <v>229</v>
       </c>
       <c r="C40" s="1">
         <v>3</v>
@@ -2650,12 +2710,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B41" t="s">
-        <v>243</v>
+      <c r="B41" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
@@ -2685,12 +2745,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B42" t="s">
-        <v>244</v>
+      <c r="B42" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="C42" s="1">
         <v>3</v>
@@ -2720,12 +2780,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B43" t="s">
-        <v>245</v>
+      <c r="B43" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
@@ -2755,12 +2815,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B44" t="s">
-        <v>246</v>
+      <c r="B44" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="C44" s="1">
         <v>3</v>
@@ -2790,12 +2850,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B45" t="s">
-        <v>247</v>
+      <c r="B45" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="C45" s="1">
         <v>4</v>
@@ -2825,12 +2885,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B46" t="s">
-        <v>248</v>
+      <c r="B46" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
@@ -2860,12 +2920,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B47" t="s">
-        <v>249</v>
+      <c r="B47" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="C47" s="1">
         <v>4</v>
@@ -2895,12 +2955,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B48" t="s">
-        <v>250</v>
+      <c r="B48" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="C48" s="1">
         <v>4</v>
@@ -2930,12 +2990,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B49" t="s">
-        <v>251</v>
+      <c r="B49" s="7" t="s">
+        <v>220</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
@@ -2965,12 +3025,12 @@
         <v>122</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B50" t="s">
-        <v>252</v>
+      <c r="B50" s="7" t="s">
+        <v>219</v>
       </c>
       <c r="C50" s="1">
         <v>5</v>
@@ -3000,12 +3060,12 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B51" t="s">
-        <v>253</v>
+      <c r="B51" s="7" t="s">
+        <v>218</v>
       </c>
       <c r="C51" s="1">
         <v>0</v>
@@ -3035,12 +3095,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B52" t="s">
-        <v>254</v>
+      <c r="B52" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="C52" s="1">
         <v>1</v>
@@ -3070,12 +3130,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B53" t="s">
-        <v>255</v>
+      <c r="B53" s="7" t="s">
+        <v>216</v>
       </c>
       <c r="C53" s="1">
         <v>0</v>
@@ -3105,12 +3165,12 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B54" t="s">
-        <v>256</v>
+      <c r="B54" s="7" t="s">
+        <v>215</v>
       </c>
       <c r="C54" s="1">
         <v>5</v>
@@ -3140,12 +3200,12 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B55" t="s">
-        <v>257</v>
+      <c r="B55" s="7" t="s">
+        <v>214</v>
       </c>
       <c r="C55" s="1">
         <v>4</v>
@@ -3163,7 +3223,7 @@
         <v>103</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>260</v>
+        <v>205</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>104</v>
@@ -3179,8 +3239,8 @@
       <c r="A56" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B56" t="s">
-        <v>258</v>
+      <c r="B56" s="7" t="s">
+        <v>213</v>
       </c>
       <c r="C56" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
debugged dense_layer, added Sequential model, and modified code for views (delete)
</commit_message>
<xml_diff>
--- a/project/core/nodes/schema.xlsx
+++ b/project/core/nodes/schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD8316B-09BF-4925-BC28-FB88B7E7952F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2411DB1E-3129-4E9F-B97B-5945627F2B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="282">
   <si>
     <t>node_name</t>
   </si>
@@ -882,13 +882,77 @@
   <si>
     <t>A boosting method that adjusts weak models 
 iteratively to minimize errors.</t>
+  </si>
+  <si>
+    <t>Input Layer</t>
+  </si>
+  <si>
+    <t>An input layer for Neural Network</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>input_layer</t>
+  </si>
+  <si>
+    <t>dense_layer</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>sequential_model</t>
+  </si>
+  <si>
+    <t>Dense Layer</t>
+  </si>
+  <si>
+    <t>Sequential Model</t>
+  </si>
+  <si>
+    <t>Neural Net hidden layer</t>
+  </si>
+  <si>
+    <t>nn_layer</t>
+  </si>
+  <si>
+    <t>nn_model</t>
+  </si>
+  <si>
+    <t>neural_network</t>
+  </si>
+  <si>
+    <t>[{"name":"input_size","type":"int","default":10}]</t>
+  </si>
+  <si>
+    <t>[{"name":"units","type":"int","default":1},
+{"name":"activation","type":"str","default":"relu"}]</t>
+  </si>
+  <si>
+    <t>["layer"]</t>
+  </si>
+  <si>
+    <t>create_input/</t>
+  </si>
+  <si>
+    <t>dense/</t>
+  </si>
+  <si>
+    <t>sequential/</t>
+  </si>
+  <si>
+    <t>["nn_model"]</t>
+  </si>
+  <si>
+    <t>["layer1","layer2","layer3"]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -901,6 +965,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -932,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -955,6 +1026,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1289,10 +1364,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3270,7 +3346,113 @@
         <v>129</v>
       </c>
     </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C57" s="1">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E57" t="s">
+        <v>264</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="I57" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K57" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C58" s="1">
+        <v>6</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E58" t="s">
+        <v>265</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="I58" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J58" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K58" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="C59" s="1">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E59" t="s">
+        <v>267</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I59" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="J59" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="K59" s="8" t="s">
+        <v>279</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sequential model updated, debugged an error with dense layer
</commit_message>
<xml_diff>
--- a/project/core/nodes/schema.xlsx
+++ b/project/core/nodes/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1mme\OneDrive\Desktop\MO\test_grad\project\core\nodes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2411DB1E-3129-4E9F-B97B-5945627F2B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28A33FA-B2F0-45EC-A74B-E4E3B406E5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{74D76D85-AA93-43E7-A272-5B691B0E160A}"/>
   </bookViews>
@@ -945,7 +945,7 @@
     <t>["nn_model"]</t>
   </si>
   <si>
-    <t>["layer1","layer2","layer3"]</t>
+    <t>["prev_node"]</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1025,9 +1025,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1366,9 +1363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E3C68DA-410F-4ABA-AB6D-2EA0770F1820}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H59" sqref="H59"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="109" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3362,22 +3359,22 @@
       <c r="E57" t="s">
         <v>264</v>
       </c>
-      <c r="F57" s="8" t="s">
+      <c r="F57" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G57" s="8" t="s">
+      <c r="G57" s="1" t="s">
         <v>273</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="I57" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J57" s="8" t="s">
+      <c r="I57" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J57" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="K57" s="9" t="s">
+      <c r="K57" s="8" t="s">
         <v>277</v>
       </c>
     </row>
@@ -3397,22 +3394,22 @@
       <c r="E58" t="s">
         <v>265</v>
       </c>
-      <c r="F58" s="8" t="s">
+      <c r="F58" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="1" t="s">
         <v>273</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="I58" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J58" s="8" t="s">
+      <c r="I58" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="J58" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="K58" s="8" t="s">
+      <c r="K58" s="1" t="s">
         <v>278</v>
       </c>
     </row>
@@ -3432,22 +3429,22 @@
       <c r="E59" t="s">
         <v>267</v>
       </c>
-      <c r="F59" s="8" t="s">
+      <c r="F59" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G59" s="1" t="s">
         <v>273</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I59" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="J59" s="8" t="s">
+      <c r="I59" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="J59" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="K59" s="8" t="s">
+      <c r="K59" s="1" t="s">
         <v>279</v>
       </c>
     </row>

</xml_diff>